<commit_message>
Updated Weekly Scoring Results
</commit_message>
<xml_diff>
--- a/AuctionDraftRecap.xlsx
+++ b/AuctionDraftRecap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ochang\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ochang\My Documents\GitHub\Whaleshit-Fantasy-Football\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3716" uniqueCount="357">
   <si>
     <t>Team</t>
   </si>
@@ -1084,6 +1084,21 @@
   </si>
   <si>
     <t>Fozzy Whittaker</t>
+  </si>
+  <si>
+    <t>Titans Defense</t>
+  </si>
+  <si>
+    <t>Vernon Davis</t>
+  </si>
+  <si>
+    <t>Ty Montgomery</t>
+  </si>
+  <si>
+    <t>Giants Defense</t>
+  </si>
+  <si>
+    <t>Mike Davis</t>
   </si>
 </sst>
 </file>
@@ -4881,10 +4896,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E541"/>
+  <dimension ref="A1:E757"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A518" workbookViewId="0">
-      <selection activeCell="B538" sqref="B538"/>
+    <sheetView tabSelected="1" topLeftCell="A694" workbookViewId="0">
+      <selection activeCell="G704" sqref="G704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14087,6 +14102,3678 @@
       </c>
       <c r="E541">
         <v>5</v>
+      </c>
+    </row>
+    <row r="542" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>4</v>
+      </c>
+      <c r="B542" t="s">
+        <v>7</v>
+      </c>
+      <c r="C542" t="s">
+        <v>24</v>
+      </c>
+      <c r="D542">
+        <v>11.5</v>
+      </c>
+      <c r="E542">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="543" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>4</v>
+      </c>
+      <c r="B543" t="s">
+        <v>5</v>
+      </c>
+      <c r="C543" t="s">
+        <v>22</v>
+      </c>
+      <c r="D543">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E543">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="544" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>4</v>
+      </c>
+      <c r="B544" t="s">
+        <v>9</v>
+      </c>
+      <c r="C544" t="s">
+        <v>22</v>
+      </c>
+      <c r="D544">
+        <v>10.8</v>
+      </c>
+      <c r="E544">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="545" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>4</v>
+      </c>
+      <c r="B545" t="s">
+        <v>6</v>
+      </c>
+      <c r="C545" t="s">
+        <v>23</v>
+      </c>
+      <c r="D545">
+        <v>1.5</v>
+      </c>
+      <c r="E545">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="546" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>4</v>
+      </c>
+      <c r="B546" t="s">
+        <v>178</v>
+      </c>
+      <c r="C546" t="s">
+        <v>23</v>
+      </c>
+      <c r="D546">
+        <v>3.8</v>
+      </c>
+      <c r="E546">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="547" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>4</v>
+      </c>
+      <c r="B547" t="s">
+        <v>11</v>
+      </c>
+      <c r="C547" t="s">
+        <v>25</v>
+      </c>
+      <c r="D547">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E547">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>4</v>
+      </c>
+      <c r="B548" t="s">
+        <v>12</v>
+      </c>
+      <c r="C548" t="s">
+        <v>326</v>
+      </c>
+      <c r="D548">
+        <v>2.6</v>
+      </c>
+      <c r="E548">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>4</v>
+      </c>
+      <c r="B549" t="s">
+        <v>352</v>
+      </c>
+      <c r="C549" t="s">
+        <v>27</v>
+      </c>
+      <c r="D549">
+        <v>6</v>
+      </c>
+      <c r="E549">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="550" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>4</v>
+      </c>
+      <c r="B550" t="s">
+        <v>13</v>
+      </c>
+      <c r="C550" t="s">
+        <v>26</v>
+      </c>
+      <c r="D550">
+        <v>9</v>
+      </c>
+      <c r="E550">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="551" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>64</v>
+      </c>
+      <c r="B551" t="s">
+        <v>78</v>
+      </c>
+      <c r="C551" t="s">
+        <v>24</v>
+      </c>
+      <c r="D551">
+        <v>23.4</v>
+      </c>
+      <c r="E551">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>64</v>
+      </c>
+      <c r="B552" t="s">
+        <v>77</v>
+      </c>
+      <c r="C552" t="s">
+        <v>22</v>
+      </c>
+      <c r="D552">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E552">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="553" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>64</v>
+      </c>
+      <c r="B553" t="s">
+        <v>83</v>
+      </c>
+      <c r="C553" t="s">
+        <v>22</v>
+      </c>
+      <c r="D553">
+        <v>12.5</v>
+      </c>
+      <c r="E553">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="554" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>64</v>
+      </c>
+      <c r="B554" t="s">
+        <v>88</v>
+      </c>
+      <c r="C554" t="s">
+        <v>23</v>
+      </c>
+      <c r="D554">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E554">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="555" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>64</v>
+      </c>
+      <c r="B555" t="s">
+        <v>337</v>
+      </c>
+      <c r="C555" t="s">
+        <v>23</v>
+      </c>
+      <c r="D555">
+        <v>2.8</v>
+      </c>
+      <c r="E555">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>64</v>
+      </c>
+      <c r="B556" t="s">
+        <v>82</v>
+      </c>
+      <c r="C556" t="s">
+        <v>25</v>
+      </c>
+      <c r="D556">
+        <v>9.4</v>
+      </c>
+      <c r="E556">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="557" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>64</v>
+      </c>
+      <c r="B557" t="s">
+        <v>84</v>
+      </c>
+      <c r="C557" t="s">
+        <v>326</v>
+      </c>
+      <c r="D557">
+        <v>19.5</v>
+      </c>
+      <c r="E557">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>64</v>
+      </c>
+      <c r="B558" t="s">
+        <v>74</v>
+      </c>
+      <c r="C558" t="s">
+        <v>27</v>
+      </c>
+      <c r="D558">
+        <v>8</v>
+      </c>
+      <c r="E558">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="559" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>64</v>
+      </c>
+      <c r="B559" t="s">
+        <v>199</v>
+      </c>
+      <c r="C559" t="s">
+        <v>26</v>
+      </c>
+      <c r="D559">
+        <v>11</v>
+      </c>
+      <c r="E559">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="560" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>67</v>
+      </c>
+      <c r="B560" t="s">
+        <v>130</v>
+      </c>
+      <c r="C560" t="s">
+        <v>24</v>
+      </c>
+      <c r="D560">
+        <v>9.6</v>
+      </c>
+      <c r="E560">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="561" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>67</v>
+      </c>
+      <c r="B561" t="s">
+        <v>127</v>
+      </c>
+      <c r="C561" t="s">
+        <v>22</v>
+      </c>
+      <c r="D561">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E561">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="562" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>67</v>
+      </c>
+      <c r="B562" t="s">
+        <v>153</v>
+      </c>
+      <c r="C562" t="s">
+        <v>22</v>
+      </c>
+      <c r="D562">
+        <v>5.3</v>
+      </c>
+      <c r="E562">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="563" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>67</v>
+      </c>
+      <c r="B563" t="s">
+        <v>126</v>
+      </c>
+      <c r="C563" t="s">
+        <v>23</v>
+      </c>
+      <c r="D563">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E563">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="564" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>67</v>
+      </c>
+      <c r="B564" t="s">
+        <v>133</v>
+      </c>
+      <c r="C564" t="s">
+        <v>23</v>
+      </c>
+      <c r="D564">
+        <v>13.8</v>
+      </c>
+      <c r="E564">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="565" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>67</v>
+      </c>
+      <c r="B565" t="s">
+        <v>347</v>
+      </c>
+      <c r="C565" t="s">
+        <v>25</v>
+      </c>
+      <c r="D565">
+        <v>1.5</v>
+      </c>
+      <c r="E565">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="566" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>67</v>
+      </c>
+      <c r="B566" t="s">
+        <v>136</v>
+      </c>
+      <c r="C566" t="s">
+        <v>326</v>
+      </c>
+      <c r="D566">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E566">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="567" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>67</v>
+      </c>
+      <c r="B567" t="s">
+        <v>119</v>
+      </c>
+      <c r="C567" t="s">
+        <v>27</v>
+      </c>
+      <c r="D567">
+        <v>0</v>
+      </c>
+      <c r="E567">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="568" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>67</v>
+      </c>
+      <c r="B568" t="s">
+        <v>123</v>
+      </c>
+      <c r="C568" t="s">
+        <v>26</v>
+      </c>
+      <c r="D568">
+        <v>12</v>
+      </c>
+      <c r="E568">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="569" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>68</v>
+      </c>
+      <c r="B569" t="s">
+        <v>151</v>
+      </c>
+      <c r="C569" t="s">
+        <v>24</v>
+      </c>
+      <c r="D569">
+        <v>21.6</v>
+      </c>
+      <c r="E569">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="570" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>68</v>
+      </c>
+      <c r="B570" t="s">
+        <v>138</v>
+      </c>
+      <c r="C570" t="s">
+        <v>22</v>
+      </c>
+      <c r="D570">
+        <v>31.8</v>
+      </c>
+      <c r="E570">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="571" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>68</v>
+      </c>
+      <c r="B571" t="s">
+        <v>139</v>
+      </c>
+      <c r="C571" t="s">
+        <v>22</v>
+      </c>
+      <c r="D571">
+        <v>20.3</v>
+      </c>
+      <c r="E571">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="572" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>68</v>
+      </c>
+      <c r="B572" t="s">
+        <v>143</v>
+      </c>
+      <c r="C572" t="s">
+        <v>23</v>
+      </c>
+      <c r="D572">
+        <v>9.1</v>
+      </c>
+      <c r="E572">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="573" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>68</v>
+      </c>
+      <c r="B573" t="s">
+        <v>149</v>
+      </c>
+      <c r="C573" t="s">
+        <v>23</v>
+      </c>
+      <c r="D573">
+        <v>1</v>
+      </c>
+      <c r="E573">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="574" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>68</v>
+      </c>
+      <c r="B574" t="s">
+        <v>144</v>
+      </c>
+      <c r="C574" t="s">
+        <v>25</v>
+      </c>
+      <c r="D574">
+        <v>2.1</v>
+      </c>
+      <c r="E574">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="575" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>68</v>
+      </c>
+      <c r="B575" t="s">
+        <v>142</v>
+      </c>
+      <c r="C575" t="s">
+        <v>326</v>
+      </c>
+      <c r="D575">
+        <v>20.5</v>
+      </c>
+      <c r="E575">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="576" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>68</v>
+      </c>
+      <c r="B576" t="s">
+        <v>150</v>
+      </c>
+      <c r="C576" t="s">
+        <v>27</v>
+      </c>
+      <c r="D576">
+        <v>11</v>
+      </c>
+      <c r="E576">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="577" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>68</v>
+      </c>
+      <c r="B577" t="s">
+        <v>288</v>
+      </c>
+      <c r="C577" t="s">
+        <v>26</v>
+      </c>
+      <c r="D577">
+        <v>6</v>
+      </c>
+      <c r="E577">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="578" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>69</v>
+      </c>
+      <c r="B578" t="s">
+        <v>162</v>
+      </c>
+      <c r="C578" t="s">
+        <v>24</v>
+      </c>
+      <c r="D578">
+        <v>21.9</v>
+      </c>
+      <c r="E578">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="579" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>69</v>
+      </c>
+      <c r="B579" t="s">
+        <v>164</v>
+      </c>
+      <c r="C579" t="s">
+        <v>22</v>
+      </c>
+      <c r="D579">
+        <v>2.7</v>
+      </c>
+      <c r="E579">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="580" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>69</v>
+      </c>
+      <c r="B580" t="s">
+        <v>167</v>
+      </c>
+      <c r="C580" t="s">
+        <v>22</v>
+      </c>
+      <c r="D580">
+        <v>13</v>
+      </c>
+      <c r="E580">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="581" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>69</v>
+      </c>
+      <c r="B581" t="s">
+        <v>154</v>
+      </c>
+      <c r="C581" t="s">
+        <v>23</v>
+      </c>
+      <c r="D581">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E581">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="582" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>69</v>
+      </c>
+      <c r="B582" t="s">
+        <v>102</v>
+      </c>
+      <c r="C582" t="s">
+        <v>23</v>
+      </c>
+      <c r="D582">
+        <v>7.7</v>
+      </c>
+      <c r="E582">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="583" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>69</v>
+      </c>
+      <c r="B583" t="s">
+        <v>157</v>
+      </c>
+      <c r="C583" t="s">
+        <v>25</v>
+      </c>
+      <c r="D583">
+        <v>22.2</v>
+      </c>
+      <c r="E583">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="584" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>69</v>
+      </c>
+      <c r="B584" t="s">
+        <v>344</v>
+      </c>
+      <c r="C584" t="s">
+        <v>326</v>
+      </c>
+      <c r="D584">
+        <v>0</v>
+      </c>
+      <c r="E584">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="585" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
+        <v>69</v>
+      </c>
+      <c r="B585" t="s">
+        <v>166</v>
+      </c>
+      <c r="C585" t="s">
+        <v>27</v>
+      </c>
+      <c r="D585">
+        <v>4</v>
+      </c>
+      <c r="E585">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="586" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>69</v>
+      </c>
+      <c r="B586" t="s">
+        <v>156</v>
+      </c>
+      <c r="C586" t="s">
+        <v>26</v>
+      </c>
+      <c r="D586">
+        <v>11</v>
+      </c>
+      <c r="E586">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="587" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>72</v>
+      </c>
+      <c r="B587" t="s">
+        <v>205</v>
+      </c>
+      <c r="C587" t="s">
+        <v>24</v>
+      </c>
+      <c r="D587">
+        <v>10.9</v>
+      </c>
+      <c r="E587">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="588" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
+        <v>72</v>
+      </c>
+      <c r="B588" t="s">
+        <v>204</v>
+      </c>
+      <c r="C588" t="s">
+        <v>22</v>
+      </c>
+      <c r="D588">
+        <v>5</v>
+      </c>
+      <c r="E588">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="589" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A589" t="s">
+        <v>72</v>
+      </c>
+      <c r="B589" t="s">
+        <v>210</v>
+      </c>
+      <c r="C589" t="s">
+        <v>22</v>
+      </c>
+      <c r="D589">
+        <v>0</v>
+      </c>
+      <c r="E589">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="590" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>72</v>
+      </c>
+      <c r="B590" t="s">
+        <v>202</v>
+      </c>
+      <c r="C590" t="s">
+        <v>23</v>
+      </c>
+      <c r="D590">
+        <v>4.5</v>
+      </c>
+      <c r="E590">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="591" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>72</v>
+      </c>
+      <c r="B591" t="s">
+        <v>203</v>
+      </c>
+      <c r="C591" t="s">
+        <v>23</v>
+      </c>
+      <c r="D591">
+        <v>7.1</v>
+      </c>
+      <c r="E591">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="592" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>72</v>
+      </c>
+      <c r="B592" t="s">
+        <v>211</v>
+      </c>
+      <c r="C592" t="s">
+        <v>25</v>
+      </c>
+      <c r="D592">
+        <v>3.6</v>
+      </c>
+      <c r="E592">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="593" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>72</v>
+      </c>
+      <c r="B593" t="s">
+        <v>344</v>
+      </c>
+      <c r="C593" t="s">
+        <v>326</v>
+      </c>
+      <c r="D593">
+        <v>0</v>
+      </c>
+      <c r="E593">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="594" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>72</v>
+      </c>
+      <c r="B594" t="s">
+        <v>213</v>
+      </c>
+      <c r="C594" t="s">
+        <v>27</v>
+      </c>
+      <c r="D594">
+        <v>11</v>
+      </c>
+      <c r="E594">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="595" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>72</v>
+      </c>
+      <c r="B595" t="s">
+        <v>214</v>
+      </c>
+      <c r="C595" t="s">
+        <v>26</v>
+      </c>
+      <c r="D595">
+        <v>7</v>
+      </c>
+      <c r="E595">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="596" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>71</v>
+      </c>
+      <c r="B596" t="s">
+        <v>194</v>
+      </c>
+      <c r="C596" t="s">
+        <v>24</v>
+      </c>
+      <c r="D596">
+        <v>12.4</v>
+      </c>
+      <c r="E596">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="597" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>71</v>
+      </c>
+      <c r="B597" t="s">
+        <v>186</v>
+      </c>
+      <c r="C597" t="s">
+        <v>22</v>
+      </c>
+      <c r="D597">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E597">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="598" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>71</v>
+      </c>
+      <c r="B598" t="s">
+        <v>187</v>
+      </c>
+      <c r="C598" t="s">
+        <v>22</v>
+      </c>
+      <c r="D598">
+        <v>12.8</v>
+      </c>
+      <c r="E598">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="599" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>71</v>
+      </c>
+      <c r="B599" t="s">
+        <v>190</v>
+      </c>
+      <c r="C599" t="s">
+        <v>23</v>
+      </c>
+      <c r="D599">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E599">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="600" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>71</v>
+      </c>
+      <c r="B600" t="s">
+        <v>195</v>
+      </c>
+      <c r="C600" t="s">
+        <v>23</v>
+      </c>
+      <c r="D600">
+        <v>8.6</v>
+      </c>
+      <c r="E600">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="601" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>71</v>
+      </c>
+      <c r="B601" t="s">
+        <v>193</v>
+      </c>
+      <c r="C601" t="s">
+        <v>25</v>
+      </c>
+      <c r="D601">
+        <v>5.9</v>
+      </c>
+      <c r="E601">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="602" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>71</v>
+      </c>
+      <c r="B602" t="s">
+        <v>198</v>
+      </c>
+      <c r="C602" t="s">
+        <v>326</v>
+      </c>
+      <c r="D602">
+        <v>7.3</v>
+      </c>
+      <c r="E602">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="603" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>71</v>
+      </c>
+      <c r="B603" t="s">
+        <v>188</v>
+      </c>
+      <c r="C603" t="s">
+        <v>27</v>
+      </c>
+      <c r="D603">
+        <v>7</v>
+      </c>
+      <c r="E603">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="604" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>71</v>
+      </c>
+      <c r="B604" t="s">
+        <v>120</v>
+      </c>
+      <c r="C604" t="s">
+        <v>26</v>
+      </c>
+      <c r="D604">
+        <v>4</v>
+      </c>
+      <c r="E604">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="605" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>28</v>
+      </c>
+      <c r="B605" t="s">
+        <v>32</v>
+      </c>
+      <c r="C605" t="s">
+        <v>24</v>
+      </c>
+      <c r="D605">
+        <v>27.2</v>
+      </c>
+      <c r="E605">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="606" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>28</v>
+      </c>
+      <c r="B606" t="s">
+        <v>36</v>
+      </c>
+      <c r="C606" t="s">
+        <v>22</v>
+      </c>
+      <c r="D606">
+        <v>7.1</v>
+      </c>
+      <c r="E606">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="607" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>28</v>
+      </c>
+      <c r="B607" t="s">
+        <v>38</v>
+      </c>
+      <c r="C607" t="s">
+        <v>22</v>
+      </c>
+      <c r="D607">
+        <v>3.5</v>
+      </c>
+      <c r="E607">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="608" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>28</v>
+      </c>
+      <c r="B608" t="s">
+        <v>29</v>
+      </c>
+      <c r="C608" t="s">
+        <v>23</v>
+      </c>
+      <c r="D608">
+        <v>12.9</v>
+      </c>
+      <c r="E608">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="609" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>28</v>
+      </c>
+      <c r="B609" t="s">
+        <v>30</v>
+      </c>
+      <c r="C609" t="s">
+        <v>23</v>
+      </c>
+      <c r="D609">
+        <v>7</v>
+      </c>
+      <c r="E609">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="610" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
+        <v>28</v>
+      </c>
+      <c r="B610" t="s">
+        <v>353</v>
+      </c>
+      <c r="C610" t="s">
+        <v>25</v>
+      </c>
+      <c r="D610">
+        <v>11</v>
+      </c>
+      <c r="E610">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="611" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>28</v>
+      </c>
+      <c r="B611" t="s">
+        <v>37</v>
+      </c>
+      <c r="C611" t="s">
+        <v>326</v>
+      </c>
+      <c r="D611">
+        <v>13.4</v>
+      </c>
+      <c r="E611">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="612" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
+        <v>28</v>
+      </c>
+      <c r="B612" t="s">
+        <v>31</v>
+      </c>
+      <c r="C612" t="s">
+        <v>27</v>
+      </c>
+      <c r="D612">
+        <v>-3</v>
+      </c>
+      <c r="E612">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="613" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>28</v>
+      </c>
+      <c r="B613" t="s">
+        <v>43</v>
+      </c>
+      <c r="C613" t="s">
+        <v>26</v>
+      </c>
+      <c r="D613">
+        <v>7</v>
+      </c>
+      <c r="E613">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="614" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>65</v>
+      </c>
+      <c r="B614" t="s">
+        <v>90</v>
+      </c>
+      <c r="C614" t="s">
+        <v>24</v>
+      </c>
+      <c r="D614">
+        <v>27</v>
+      </c>
+      <c r="E614">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="615" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
+        <v>65</v>
+      </c>
+      <c r="B615" t="s">
+        <v>95</v>
+      </c>
+      <c r="C615" t="s">
+        <v>22</v>
+      </c>
+      <c r="D615">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E615">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="616" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A616" t="s">
+        <v>65</v>
+      </c>
+      <c r="B616" t="s">
+        <v>96</v>
+      </c>
+      <c r="C616" t="s">
+        <v>22</v>
+      </c>
+      <c r="D616">
+        <v>5.2</v>
+      </c>
+      <c r="E616">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="617" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>65</v>
+      </c>
+      <c r="B617" t="s">
+        <v>91</v>
+      </c>
+      <c r="C617" t="s">
+        <v>23</v>
+      </c>
+      <c r="D617">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E617">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="618" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A618" t="s">
+        <v>65</v>
+      </c>
+      <c r="B618" t="s">
+        <v>92</v>
+      </c>
+      <c r="C618" t="s">
+        <v>23</v>
+      </c>
+      <c r="D618">
+        <v>4.8</v>
+      </c>
+      <c r="E618">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="619" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
+        <v>65</v>
+      </c>
+      <c r="B619" t="s">
+        <v>333</v>
+      </c>
+      <c r="C619" t="s">
+        <v>25</v>
+      </c>
+      <c r="D619">
+        <v>3.6</v>
+      </c>
+      <c r="E619">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="620" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
+        <v>65</v>
+      </c>
+      <c r="B620" t="s">
+        <v>350</v>
+      </c>
+      <c r="C620" t="s">
+        <v>326</v>
+      </c>
+      <c r="D620">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E620">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="621" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
+        <v>65</v>
+      </c>
+      <c r="B621" t="s">
+        <v>20</v>
+      </c>
+      <c r="C621" t="s">
+        <v>27</v>
+      </c>
+      <c r="D621">
+        <v>6</v>
+      </c>
+      <c r="E621">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="622" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
+        <v>65</v>
+      </c>
+      <c r="B622" t="s">
+        <v>98</v>
+      </c>
+      <c r="C622" t="s">
+        <v>26</v>
+      </c>
+      <c r="D622">
+        <v>13</v>
+      </c>
+      <c r="E622">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="623" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>45</v>
+      </c>
+      <c r="B623" t="s">
+        <v>60</v>
+      </c>
+      <c r="C623" t="s">
+        <v>24</v>
+      </c>
+      <c r="D623">
+        <v>8.9</v>
+      </c>
+      <c r="E623">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="624" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A624" t="s">
+        <v>45</v>
+      </c>
+      <c r="B624" t="s">
+        <v>56</v>
+      </c>
+      <c r="C624" t="s">
+        <v>22</v>
+      </c>
+      <c r="D624">
+        <v>3.6</v>
+      </c>
+      <c r="E624">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="625" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>45</v>
+      </c>
+      <c r="B625" t="s">
+        <v>57</v>
+      </c>
+      <c r="C625" t="s">
+        <v>22</v>
+      </c>
+      <c r="D625">
+        <v>24.3</v>
+      </c>
+      <c r="E625">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="626" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>45</v>
+      </c>
+      <c r="B626" t="s">
+        <v>47</v>
+      </c>
+      <c r="C626" t="s">
+        <v>23</v>
+      </c>
+      <c r="D626">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E626">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="627" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A627" t="s">
+        <v>45</v>
+      </c>
+      <c r="B627" t="s">
+        <v>52</v>
+      </c>
+      <c r="C627" t="s">
+        <v>23</v>
+      </c>
+      <c r="D627">
+        <v>4</v>
+      </c>
+      <c r="E627">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="628" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
+        <v>45</v>
+      </c>
+      <c r="B628" t="s">
+        <v>51</v>
+      </c>
+      <c r="C628" t="s">
+        <v>25</v>
+      </c>
+      <c r="D628">
+        <v>4.8</v>
+      </c>
+      <c r="E628">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="629" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
+        <v>45</v>
+      </c>
+      <c r="B629" t="s">
+        <v>53</v>
+      </c>
+      <c r="C629" t="s">
+        <v>326</v>
+      </c>
+      <c r="D629">
+        <v>5.5</v>
+      </c>
+      <c r="E629">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="630" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A630" t="s">
+        <v>45</v>
+      </c>
+      <c r="B630" t="s">
+        <v>54</v>
+      </c>
+      <c r="C630" t="s">
+        <v>27</v>
+      </c>
+      <c r="D630">
+        <v>4</v>
+      </c>
+      <c r="E630">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="631" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
+        <v>45</v>
+      </c>
+      <c r="B631" t="s">
+        <v>61</v>
+      </c>
+      <c r="C631" t="s">
+        <v>26</v>
+      </c>
+      <c r="D631">
+        <v>8</v>
+      </c>
+      <c r="E631">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="632" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>66</v>
+      </c>
+      <c r="B632" t="s">
+        <v>109</v>
+      </c>
+      <c r="C632" t="s">
+        <v>24</v>
+      </c>
+      <c r="D632">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E632">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="633" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A633" t="s">
+        <v>66</v>
+      </c>
+      <c r="B633" t="s">
+        <v>106</v>
+      </c>
+      <c r="C633" t="s">
+        <v>22</v>
+      </c>
+      <c r="D633">
+        <v>29.8</v>
+      </c>
+      <c r="E633">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="634" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>66</v>
+      </c>
+      <c r="B634" t="s">
+        <v>263</v>
+      </c>
+      <c r="C634" t="s">
+        <v>22</v>
+      </c>
+      <c r="D634">
+        <v>10</v>
+      </c>
+      <c r="E634">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="635" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A635" t="s">
+        <v>66</v>
+      </c>
+      <c r="B635" t="s">
+        <v>107</v>
+      </c>
+      <c r="C635" t="s">
+        <v>23</v>
+      </c>
+      <c r="D635">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E635">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="636" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A636" t="s">
+        <v>66</v>
+      </c>
+      <c r="B636" t="s">
+        <v>110</v>
+      </c>
+      <c r="C636" t="s">
+        <v>23</v>
+      </c>
+      <c r="D636">
+        <v>23.5</v>
+      </c>
+      <c r="E636">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="637" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A637" t="s">
+        <v>66</v>
+      </c>
+      <c r="B637" t="s">
+        <v>111</v>
+      </c>
+      <c r="C637" t="s">
+        <v>25</v>
+      </c>
+      <c r="D637">
+        <v>8.9</v>
+      </c>
+      <c r="E637">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="638" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A638" t="s">
+        <v>66</v>
+      </c>
+      <c r="B638" t="s">
+        <v>108</v>
+      </c>
+      <c r="C638" t="s">
+        <v>326</v>
+      </c>
+      <c r="D638">
+        <v>7.1</v>
+      </c>
+      <c r="E638">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="639" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A639" t="s">
+        <v>66</v>
+      </c>
+      <c r="B639" t="s">
+        <v>339</v>
+      </c>
+      <c r="C639" t="s">
+        <v>27</v>
+      </c>
+      <c r="D639">
+        <v>-4</v>
+      </c>
+      <c r="E639">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="640" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
+        <v>66</v>
+      </c>
+      <c r="B640" t="s">
+        <v>340</v>
+      </c>
+      <c r="C640" t="s">
+        <v>26</v>
+      </c>
+      <c r="D640">
+        <v>11</v>
+      </c>
+      <c r="E640">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="641" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A641" t="s">
+        <v>70</v>
+      </c>
+      <c r="B641" t="s">
+        <v>173</v>
+      </c>
+      <c r="C641" t="s">
+        <v>24</v>
+      </c>
+      <c r="D641">
+        <v>12.5</v>
+      </c>
+      <c r="E641">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="642" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A642" t="s">
+        <v>70</v>
+      </c>
+      <c r="B642" t="s">
+        <v>171</v>
+      </c>
+      <c r="C642" t="s">
+        <v>22</v>
+      </c>
+      <c r="D642">
+        <v>9.4</v>
+      </c>
+      <c r="E642">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="643" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A643" t="s">
+        <v>70</v>
+      </c>
+      <c r="B643" t="s">
+        <v>174</v>
+      </c>
+      <c r="C643" t="s">
+        <v>22</v>
+      </c>
+      <c r="D643">
+        <v>10.7</v>
+      </c>
+      <c r="E643">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="644" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A644" t="s">
+        <v>70</v>
+      </c>
+      <c r="B644" t="s">
+        <v>177</v>
+      </c>
+      <c r="C644" t="s">
+        <v>23</v>
+      </c>
+      <c r="D644">
+        <v>3.1</v>
+      </c>
+      <c r="E644">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="645" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A645" t="s">
+        <v>70</v>
+      </c>
+      <c r="B645" t="s">
+        <v>266</v>
+      </c>
+      <c r="C645" t="s">
+        <v>23</v>
+      </c>
+      <c r="D645">
+        <v>0</v>
+      </c>
+      <c r="E645">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="646" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A646" t="s">
+        <v>70</v>
+      </c>
+      <c r="B646" t="s">
+        <v>179</v>
+      </c>
+      <c r="C646" t="s">
+        <v>25</v>
+      </c>
+      <c r="D646">
+        <v>3.2</v>
+      </c>
+      <c r="E646">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="647" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A647" t="s">
+        <v>70</v>
+      </c>
+      <c r="B647" t="s">
+        <v>341</v>
+      </c>
+      <c r="C647" t="s">
+        <v>326</v>
+      </c>
+      <c r="D647">
+        <v>19.8</v>
+      </c>
+      <c r="E647">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="648" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A648" t="s">
+        <v>70</v>
+      </c>
+      <c r="B648" t="s">
+        <v>172</v>
+      </c>
+      <c r="C648" t="s">
+        <v>27</v>
+      </c>
+      <c r="D648">
+        <v>-6</v>
+      </c>
+      <c r="E648">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="649" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A649" t="s">
+        <v>70</v>
+      </c>
+      <c r="B649" t="s">
+        <v>170</v>
+      </c>
+      <c r="C649" t="s">
+        <v>26</v>
+      </c>
+      <c r="D649">
+        <v>10</v>
+      </c>
+      <c r="E649">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="650" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A650" t="s">
+        <v>4</v>
+      </c>
+      <c r="B650" t="s">
+        <v>7</v>
+      </c>
+      <c r="C650" t="s">
+        <v>24</v>
+      </c>
+      <c r="D650">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E650">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="651" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A651" t="s">
+        <v>4</v>
+      </c>
+      <c r="B651" t="s">
+        <v>9</v>
+      </c>
+      <c r="C651" t="s">
+        <v>22</v>
+      </c>
+      <c r="D651">
+        <v>14.3</v>
+      </c>
+      <c r="E651">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="652" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A652" t="s">
+        <v>4</v>
+      </c>
+      <c r="B652" t="s">
+        <v>14</v>
+      </c>
+      <c r="C652" t="s">
+        <v>22</v>
+      </c>
+      <c r="D652">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E652">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="653" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A653" t="s">
+        <v>4</v>
+      </c>
+      <c r="B653" t="s">
+        <v>6</v>
+      </c>
+      <c r="C653" t="s">
+        <v>23</v>
+      </c>
+      <c r="D653">
+        <v>10</v>
+      </c>
+      <c r="E653">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="654" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A654" t="s">
+        <v>4</v>
+      </c>
+      <c r="B654" t="s">
+        <v>178</v>
+      </c>
+      <c r="C654" t="s">
+        <v>23</v>
+      </c>
+      <c r="D654">
+        <v>4</v>
+      </c>
+      <c r="E654">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="655" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A655" t="s">
+        <v>4</v>
+      </c>
+      <c r="B655" t="s">
+        <v>11</v>
+      </c>
+      <c r="C655" t="s">
+        <v>25</v>
+      </c>
+      <c r="D655">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E655">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="656" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A656" t="s">
+        <v>4</v>
+      </c>
+      <c r="B656" t="s">
+        <v>354</v>
+      </c>
+      <c r="C656" t="s">
+        <v>326</v>
+      </c>
+      <c r="D656">
+        <v>12.6</v>
+      </c>
+      <c r="E656">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="657" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A657" t="s">
+        <v>4</v>
+      </c>
+      <c r="B657" t="s">
+        <v>105</v>
+      </c>
+      <c r="C657" t="s">
+        <v>27</v>
+      </c>
+      <c r="D657">
+        <v>17</v>
+      </c>
+      <c r="E657">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="658" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A658" t="s">
+        <v>4</v>
+      </c>
+      <c r="B658" t="s">
+        <v>13</v>
+      </c>
+      <c r="C658" t="s">
+        <v>26</v>
+      </c>
+      <c r="D658">
+        <v>6</v>
+      </c>
+      <c r="E658">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="659" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A659" t="s">
+        <v>70</v>
+      </c>
+      <c r="B659" t="s">
+        <v>176</v>
+      </c>
+      <c r="C659" t="s">
+        <v>24</v>
+      </c>
+      <c r="D659">
+        <v>14.6</v>
+      </c>
+      <c r="E659">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="660" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A660" t="s">
+        <v>70</v>
+      </c>
+      <c r="B660" t="s">
+        <v>171</v>
+      </c>
+      <c r="C660" t="s">
+        <v>22</v>
+      </c>
+      <c r="D660">
+        <v>30.1</v>
+      </c>
+      <c r="E660">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="661" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A661" t="s">
+        <v>70</v>
+      </c>
+      <c r="B661" t="s">
+        <v>174</v>
+      </c>
+      <c r="C661" t="s">
+        <v>22</v>
+      </c>
+      <c r="D661">
+        <v>0</v>
+      </c>
+      <c r="E661">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="662" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A662" t="s">
+        <v>70</v>
+      </c>
+      <c r="B662" t="s">
+        <v>177</v>
+      </c>
+      <c r="C662" t="s">
+        <v>23</v>
+      </c>
+      <c r="D662">
+        <v>6.9</v>
+      </c>
+      <c r="E662">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="663" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A663" t="s">
+        <v>70</v>
+      </c>
+      <c r="B663" t="s">
+        <v>341</v>
+      </c>
+      <c r="C663" t="s">
+        <v>23</v>
+      </c>
+      <c r="D663">
+        <v>1.8</v>
+      </c>
+      <c r="E663">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="664" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A664" t="s">
+        <v>70</v>
+      </c>
+      <c r="B664" t="s">
+        <v>179</v>
+      </c>
+      <c r="C664" t="s">
+        <v>25</v>
+      </c>
+      <c r="D664">
+        <v>2.4</v>
+      </c>
+      <c r="E664">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="665" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A665" t="s">
+        <v>70</v>
+      </c>
+      <c r="B665" t="s">
+        <v>336</v>
+      </c>
+      <c r="C665" t="s">
+        <v>326</v>
+      </c>
+      <c r="D665">
+        <v>4.8</v>
+      </c>
+      <c r="E665">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="666" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A666" t="s">
+        <v>70</v>
+      </c>
+      <c r="B666" t="s">
+        <v>355</v>
+      </c>
+      <c r="C666" t="s">
+        <v>27</v>
+      </c>
+      <c r="D666">
+        <v>20</v>
+      </c>
+      <c r="E666">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="667" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A667" t="s">
+        <v>70</v>
+      </c>
+      <c r="B667" t="s">
+        <v>170</v>
+      </c>
+      <c r="C667" t="s">
+        <v>26</v>
+      </c>
+      <c r="D667">
+        <v>3</v>
+      </c>
+      <c r="E667">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="668" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A668" t="s">
+        <v>68</v>
+      </c>
+      <c r="B668" t="s">
+        <v>151</v>
+      </c>
+      <c r="C668" t="s">
+        <v>24</v>
+      </c>
+      <c r="D668">
+        <v>13.7</v>
+      </c>
+      <c r="E668">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="669" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A669" t="s">
+        <v>68</v>
+      </c>
+      <c r="B669" t="s">
+        <v>138</v>
+      </c>
+      <c r="C669" t="s">
+        <v>22</v>
+      </c>
+      <c r="D669">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="E669">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="670" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A670" t="s">
+        <v>68</v>
+      </c>
+      <c r="B670" t="s">
+        <v>139</v>
+      </c>
+      <c r="C670" t="s">
+        <v>22</v>
+      </c>
+      <c r="D670">
+        <v>5.5</v>
+      </c>
+      <c r="E670">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="671" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A671" t="s">
+        <v>68</v>
+      </c>
+      <c r="B671" t="s">
+        <v>143</v>
+      </c>
+      <c r="C671" t="s">
+        <v>23</v>
+      </c>
+      <c r="D671">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E671">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="672" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A672" t="s">
+        <v>68</v>
+      </c>
+      <c r="B672" t="s">
+        <v>149</v>
+      </c>
+      <c r="C672" t="s">
+        <v>23</v>
+      </c>
+      <c r="D672">
+        <v>15.6</v>
+      </c>
+      <c r="E672">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="673" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A673" t="s">
+        <v>68</v>
+      </c>
+      <c r="B673" t="s">
+        <v>144</v>
+      </c>
+      <c r="C673" t="s">
+        <v>25</v>
+      </c>
+      <c r="D673">
+        <v>14.4</v>
+      </c>
+      <c r="E673">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="674" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A674" t="s">
+        <v>68</v>
+      </c>
+      <c r="B674" t="s">
+        <v>345</v>
+      </c>
+      <c r="C674" t="s">
+        <v>326</v>
+      </c>
+      <c r="D674">
+        <v>16.3</v>
+      </c>
+      <c r="E674">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="675" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A675" t="s">
+        <v>68</v>
+      </c>
+      <c r="B675" t="s">
+        <v>150</v>
+      </c>
+      <c r="C675" t="s">
+        <v>27</v>
+      </c>
+      <c r="D675">
+        <v>7</v>
+      </c>
+      <c r="E675">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="676" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A676" t="s">
+        <v>68</v>
+      </c>
+      <c r="B676" t="s">
+        <v>288</v>
+      </c>
+      <c r="C676" t="s">
+        <v>26</v>
+      </c>
+      <c r="D676">
+        <v>12</v>
+      </c>
+      <c r="E676">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="677" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A677" t="s">
+        <v>72</v>
+      </c>
+      <c r="B677" t="s">
+        <v>205</v>
+      </c>
+      <c r="C677" t="s">
+        <v>24</v>
+      </c>
+      <c r="D677">
+        <v>13.1</v>
+      </c>
+      <c r="E677">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="678" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A678" t="s">
+        <v>72</v>
+      </c>
+      <c r="B678" t="s">
+        <v>204</v>
+      </c>
+      <c r="C678" t="s">
+        <v>22</v>
+      </c>
+      <c r="D678">
+        <v>10</v>
+      </c>
+      <c r="E678">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="679" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A679" t="s">
+        <v>72</v>
+      </c>
+      <c r="B679" t="s">
+        <v>210</v>
+      </c>
+      <c r="C679" t="s">
+        <v>22</v>
+      </c>
+      <c r="D679">
+        <v>0</v>
+      </c>
+      <c r="E679">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="680" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A680" t="s">
+        <v>72</v>
+      </c>
+      <c r="B680" t="s">
+        <v>202</v>
+      </c>
+      <c r="C680" t="s">
+        <v>23</v>
+      </c>
+      <c r="D680">
+        <v>11.9</v>
+      </c>
+      <c r="E680">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="681" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A681" t="s">
+        <v>72</v>
+      </c>
+      <c r="B681" t="s">
+        <v>203</v>
+      </c>
+      <c r="C681" t="s">
+        <v>23</v>
+      </c>
+      <c r="D681">
+        <v>3.6</v>
+      </c>
+      <c r="E681">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="682" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A682" t="s">
+        <v>72</v>
+      </c>
+      <c r="B682" t="s">
+        <v>211</v>
+      </c>
+      <c r="C682" t="s">
+        <v>25</v>
+      </c>
+      <c r="D682">
+        <v>4</v>
+      </c>
+      <c r="E682">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="683" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A683" t="s">
+        <v>72</v>
+      </c>
+      <c r="B683" t="s">
+        <v>208</v>
+      </c>
+      <c r="C683" t="s">
+        <v>326</v>
+      </c>
+      <c r="D683">
+        <v>1.8</v>
+      </c>
+      <c r="E683">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="684" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A684" t="s">
+        <v>72</v>
+      </c>
+      <c r="B684" t="s">
+        <v>213</v>
+      </c>
+      <c r="C684" t="s">
+        <v>27</v>
+      </c>
+      <c r="D684">
+        <v>6</v>
+      </c>
+      <c r="E684">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="685" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A685" t="s">
+        <v>72</v>
+      </c>
+      <c r="B685" t="s">
+        <v>344</v>
+      </c>
+      <c r="C685" t="s">
+        <v>26</v>
+      </c>
+      <c r="D685">
+        <v>0</v>
+      </c>
+      <c r="E685">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="686" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A686" t="s">
+        <v>28</v>
+      </c>
+      <c r="B686" t="s">
+        <v>32</v>
+      </c>
+      <c r="C686" t="s">
+        <v>24</v>
+      </c>
+      <c r="D686">
+        <v>18.2</v>
+      </c>
+      <c r="E686">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="687" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A687" t="s">
+        <v>28</v>
+      </c>
+      <c r="B687" t="s">
+        <v>36</v>
+      </c>
+      <c r="C687" t="s">
+        <v>22</v>
+      </c>
+      <c r="D687">
+        <v>16.7</v>
+      </c>
+      <c r="E687">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="688" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A688" t="s">
+        <v>28</v>
+      </c>
+      <c r="B688" t="s">
+        <v>38</v>
+      </c>
+      <c r="C688" t="s">
+        <v>22</v>
+      </c>
+      <c r="D688">
+        <v>10.9</v>
+      </c>
+      <c r="E688">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="689" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A689" t="s">
+        <v>28</v>
+      </c>
+      <c r="B689" t="s">
+        <v>29</v>
+      </c>
+      <c r="C689" t="s">
+        <v>23</v>
+      </c>
+      <c r="D689">
+        <v>2.9</v>
+      </c>
+      <c r="E689">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="690" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A690" t="s">
+        <v>28</v>
+      </c>
+      <c r="B690" t="s">
+        <v>30</v>
+      </c>
+      <c r="C690" t="s">
+        <v>23</v>
+      </c>
+      <c r="D690">
+        <v>3.9</v>
+      </c>
+      <c r="E690">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="691" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A691" t="s">
+        <v>28</v>
+      </c>
+      <c r="B691" t="s">
+        <v>353</v>
+      </c>
+      <c r="C691" t="s">
+        <v>25</v>
+      </c>
+      <c r="D691">
+        <v>7.9</v>
+      </c>
+      <c r="E691">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="692" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A692" t="s">
+        <v>28</v>
+      </c>
+      <c r="B692" t="s">
+        <v>37</v>
+      </c>
+      <c r="C692" t="s">
+        <v>326</v>
+      </c>
+      <c r="D692">
+        <v>3.3</v>
+      </c>
+      <c r="E692">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="693" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A693" t="s">
+        <v>28</v>
+      </c>
+      <c r="B693" t="s">
+        <v>31</v>
+      </c>
+      <c r="C693" t="s">
+        <v>27</v>
+      </c>
+      <c r="D693">
+        <v>6</v>
+      </c>
+      <c r="E693">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="694" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A694" t="s">
+        <v>28</v>
+      </c>
+      <c r="B694" t="s">
+        <v>43</v>
+      </c>
+      <c r="C694" t="s">
+        <v>26</v>
+      </c>
+      <c r="D694">
+        <v>8</v>
+      </c>
+      <c r="E694">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="695" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A695" t="s">
+        <v>67</v>
+      </c>
+      <c r="B695" t="s">
+        <v>125</v>
+      </c>
+      <c r="C695" t="s">
+        <v>24</v>
+      </c>
+      <c r="D695">
+        <v>21.5</v>
+      </c>
+      <c r="E695">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="696" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A696" t="s">
+        <v>67</v>
+      </c>
+      <c r="B696" t="s">
+        <v>136</v>
+      </c>
+      <c r="C696" t="s">
+        <v>22</v>
+      </c>
+      <c r="D696">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E696">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="697" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A697" t="s">
+        <v>67</v>
+      </c>
+      <c r="B697" t="s">
+        <v>153</v>
+      </c>
+      <c r="C697" t="s">
+        <v>22</v>
+      </c>
+      <c r="D697">
+        <v>14.7</v>
+      </c>
+      <c r="E697">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="698" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A698" t="s">
+        <v>67</v>
+      </c>
+      <c r="B698" t="s">
+        <v>126</v>
+      </c>
+      <c r="C698" t="s">
+        <v>23</v>
+      </c>
+      <c r="D698">
+        <v>22.9</v>
+      </c>
+      <c r="E698">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="699" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A699" t="s">
+        <v>67</v>
+      </c>
+      <c r="B699" t="s">
+        <v>133</v>
+      </c>
+      <c r="C699" t="s">
+        <v>23</v>
+      </c>
+      <c r="D699">
+        <v>13</v>
+      </c>
+      <c r="E699">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="700" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A700" t="s">
+        <v>67</v>
+      </c>
+      <c r="B700" t="s">
+        <v>347</v>
+      </c>
+      <c r="C700" t="s">
+        <v>25</v>
+      </c>
+      <c r="D700">
+        <v>0.7</v>
+      </c>
+      <c r="E700">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="701" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A701" t="s">
+        <v>67</v>
+      </c>
+      <c r="B701" t="s">
+        <v>129</v>
+      </c>
+      <c r="C701" t="s">
+        <v>326</v>
+      </c>
+      <c r="D701">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E701">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="702" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A702" t="s">
+        <v>67</v>
+      </c>
+      <c r="B702" t="s">
+        <v>119</v>
+      </c>
+      <c r="C702" t="s">
+        <v>27</v>
+      </c>
+      <c r="D702">
+        <v>5</v>
+      </c>
+      <c r="E702">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="703" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A703" t="s">
+        <v>67</v>
+      </c>
+      <c r="B703" t="s">
+        <v>123</v>
+      </c>
+      <c r="C703" t="s">
+        <v>26</v>
+      </c>
+      <c r="D703">
+        <v>10</v>
+      </c>
+      <c r="E703">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="704" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A704" t="s">
+        <v>64</v>
+      </c>
+      <c r="B704" t="s">
+        <v>78</v>
+      </c>
+      <c r="C704" t="s">
+        <v>24</v>
+      </c>
+      <c r="D704">
+        <v>27.8</v>
+      </c>
+      <c r="E704">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="705" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A705" t="s">
+        <v>64</v>
+      </c>
+      <c r="B705" t="s">
+        <v>83</v>
+      </c>
+      <c r="C705" t="s">
+        <v>22</v>
+      </c>
+      <c r="D705">
+        <v>18.7</v>
+      </c>
+      <c r="E705">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="706" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A706" t="s">
+        <v>64</v>
+      </c>
+      <c r="B706" t="s">
+        <v>84</v>
+      </c>
+      <c r="C706" t="s">
+        <v>22</v>
+      </c>
+      <c r="D706">
+        <v>0.7</v>
+      </c>
+      <c r="E706">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="707" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A707" t="s">
+        <v>64</v>
+      </c>
+      <c r="B707" t="s">
+        <v>79</v>
+      </c>
+      <c r="C707" t="s">
+        <v>23</v>
+      </c>
+      <c r="D707">
+        <v>21.6</v>
+      </c>
+      <c r="E707">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="708" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A708" t="s">
+        <v>64</v>
+      </c>
+      <c r="B708" t="s">
+        <v>88</v>
+      </c>
+      <c r="C708" t="s">
+        <v>23</v>
+      </c>
+      <c r="D708">
+        <v>12</v>
+      </c>
+      <c r="E708">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="709" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A709" t="s">
+        <v>64</v>
+      </c>
+      <c r="B709" t="s">
+        <v>297</v>
+      </c>
+      <c r="C709" t="s">
+        <v>25</v>
+      </c>
+      <c r="D709">
+        <v>1.6</v>
+      </c>
+      <c r="E709">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="710" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A710" t="s">
+        <v>64</v>
+      </c>
+      <c r="B710" t="s">
+        <v>86</v>
+      </c>
+      <c r="C710" t="s">
+        <v>326</v>
+      </c>
+      <c r="D710">
+        <v>27.6</v>
+      </c>
+      <c r="E710">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="711" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A711" t="s">
+        <v>64</v>
+      </c>
+      <c r="B711" t="s">
+        <v>74</v>
+      </c>
+      <c r="C711" t="s">
+        <v>27</v>
+      </c>
+      <c r="D711">
+        <v>10</v>
+      </c>
+      <c r="E711">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="712" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A712" t="s">
+        <v>64</v>
+      </c>
+      <c r="B712" t="s">
+        <v>199</v>
+      </c>
+      <c r="C712" t="s">
+        <v>26</v>
+      </c>
+      <c r="D712">
+        <v>8</v>
+      </c>
+      <c r="E712">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="713" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A713" t="s">
+        <v>69</v>
+      </c>
+      <c r="B713" t="s">
+        <v>162</v>
+      </c>
+      <c r="C713" t="s">
+        <v>24</v>
+      </c>
+      <c r="D713">
+        <v>20.3</v>
+      </c>
+      <c r="E713">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="714" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A714" t="s">
+        <v>69</v>
+      </c>
+      <c r="B714" t="s">
+        <v>158</v>
+      </c>
+      <c r="C714" t="s">
+        <v>22</v>
+      </c>
+      <c r="D714">
+        <v>12.2</v>
+      </c>
+      <c r="E714">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="715" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A715" t="s">
+        <v>69</v>
+      </c>
+      <c r="B715" t="s">
+        <v>167</v>
+      </c>
+      <c r="C715" t="s">
+        <v>22</v>
+      </c>
+      <c r="D715">
+        <v>25.4</v>
+      </c>
+      <c r="E715">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="716" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A716" t="s">
+        <v>69</v>
+      </c>
+      <c r="B716" t="s">
+        <v>154</v>
+      </c>
+      <c r="C716" t="s">
+        <v>23</v>
+      </c>
+      <c r="D716">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E716">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="717" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A717" t="s">
+        <v>69</v>
+      </c>
+      <c r="B717" t="s">
+        <v>102</v>
+      </c>
+      <c r="C717" t="s">
+        <v>23</v>
+      </c>
+      <c r="D717">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E717">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="718" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A718" t="s">
+        <v>69</v>
+      </c>
+      <c r="B718" t="s">
+        <v>157</v>
+      </c>
+      <c r="C718" t="s">
+        <v>25</v>
+      </c>
+      <c r="D718">
+        <v>15.3</v>
+      </c>
+      <c r="E718">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="719" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A719" t="s">
+        <v>69</v>
+      </c>
+      <c r="B719" t="s">
+        <v>161</v>
+      </c>
+      <c r="C719" t="s">
+        <v>326</v>
+      </c>
+      <c r="D719">
+        <v>4.5</v>
+      </c>
+      <c r="E719">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="720" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A720" t="s">
+        <v>69</v>
+      </c>
+      <c r="B720" t="s">
+        <v>166</v>
+      </c>
+      <c r="C720" t="s">
+        <v>27</v>
+      </c>
+      <c r="D720">
+        <v>0</v>
+      </c>
+      <c r="E720">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="721" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A721" t="s">
+        <v>69</v>
+      </c>
+      <c r="B721" t="s">
+        <v>156</v>
+      </c>
+      <c r="C721" t="s">
+        <v>26</v>
+      </c>
+      <c r="D721">
+        <v>14</v>
+      </c>
+      <c r="E721">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="722" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A722" t="s">
+        <v>45</v>
+      </c>
+      <c r="B722" t="s">
+        <v>60</v>
+      </c>
+      <c r="C722" t="s">
+        <v>24</v>
+      </c>
+      <c r="D722">
+        <v>17.3</v>
+      </c>
+      <c r="E722">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="723" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A723" t="s">
+        <v>45</v>
+      </c>
+      <c r="B723" t="s">
+        <v>56</v>
+      </c>
+      <c r="C723" t="s">
+        <v>22</v>
+      </c>
+      <c r="D723">
+        <v>13.9</v>
+      </c>
+      <c r="E723">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="724" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A724" t="s">
+        <v>45</v>
+      </c>
+      <c r="B724" t="s">
+        <v>57</v>
+      </c>
+      <c r="C724" t="s">
+        <v>22</v>
+      </c>
+      <c r="D724">
+        <v>1</v>
+      </c>
+      <c r="E724">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="725" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A725" t="s">
+        <v>45</v>
+      </c>
+      <c r="B725" t="s">
+        <v>47</v>
+      </c>
+      <c r="C725" t="s">
+        <v>23</v>
+      </c>
+      <c r="D725">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E725">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="726" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A726" t="s">
+        <v>45</v>
+      </c>
+      <c r="B726" t="s">
+        <v>52</v>
+      </c>
+      <c r="C726" t="s">
+        <v>23</v>
+      </c>
+      <c r="D726">
+        <v>8.6</v>
+      </c>
+      <c r="E726">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="727" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A727" t="s">
+        <v>45</v>
+      </c>
+      <c r="B727" t="s">
+        <v>51</v>
+      </c>
+      <c r="C727" t="s">
+        <v>25</v>
+      </c>
+      <c r="D727">
+        <v>0.5</v>
+      </c>
+      <c r="E727">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="728" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A728" t="s">
+        <v>45</v>
+      </c>
+      <c r="B728" t="s">
+        <v>53</v>
+      </c>
+      <c r="C728" t="s">
+        <v>326</v>
+      </c>
+      <c r="D728">
+        <v>3.5</v>
+      </c>
+      <c r="E728">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="729" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A729" t="s">
+        <v>45</v>
+      </c>
+      <c r="B729" t="s">
+        <v>54</v>
+      </c>
+      <c r="C729" t="s">
+        <v>27</v>
+      </c>
+      <c r="D729">
+        <v>2</v>
+      </c>
+      <c r="E729">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="730" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A730" t="s">
+        <v>45</v>
+      </c>
+      <c r="B730" t="s">
+        <v>61</v>
+      </c>
+      <c r="C730" t="s">
+        <v>26</v>
+      </c>
+      <c r="D730">
+        <v>11</v>
+      </c>
+      <c r="E730">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="731" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A731" t="s">
+        <v>71</v>
+      </c>
+      <c r="B731" t="s">
+        <v>194</v>
+      </c>
+      <c r="C731" t="s">
+        <v>24</v>
+      </c>
+      <c r="D731">
+        <v>14.5</v>
+      </c>
+      <c r="E731">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="732" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A732" t="s">
+        <v>71</v>
+      </c>
+      <c r="B732" t="s">
+        <v>186</v>
+      </c>
+      <c r="C732" t="s">
+        <v>22</v>
+      </c>
+      <c r="D732">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E732">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="733" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A733" t="s">
+        <v>71</v>
+      </c>
+      <c r="B733" t="s">
+        <v>187</v>
+      </c>
+      <c r="C733" t="s">
+        <v>22</v>
+      </c>
+      <c r="D733">
+        <v>14.9</v>
+      </c>
+      <c r="E733">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="734" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A734" t="s">
+        <v>71</v>
+      </c>
+      <c r="B734" t="s">
+        <v>190</v>
+      </c>
+      <c r="C734" t="s">
+        <v>23</v>
+      </c>
+      <c r="D734">
+        <v>7</v>
+      </c>
+      <c r="E734">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="735" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A735" t="s">
+        <v>71</v>
+      </c>
+      <c r="B735" t="s">
+        <v>198</v>
+      </c>
+      <c r="C735" t="s">
+        <v>23</v>
+      </c>
+      <c r="D735">
+        <v>9.4</v>
+      </c>
+      <c r="E735">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="736" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A736" t="s">
+        <v>71</v>
+      </c>
+      <c r="B736" t="s">
+        <v>193</v>
+      </c>
+      <c r="C736" t="s">
+        <v>25</v>
+      </c>
+      <c r="D736">
+        <v>6.6</v>
+      </c>
+      <c r="E736">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="737" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A737" t="s">
+        <v>71</v>
+      </c>
+      <c r="B737" t="s">
+        <v>189</v>
+      </c>
+      <c r="C737" t="s">
+        <v>326</v>
+      </c>
+      <c r="D737">
+        <v>14.7</v>
+      </c>
+      <c r="E737">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="738" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A738" t="s">
+        <v>71</v>
+      </c>
+      <c r="B738" t="s">
+        <v>188</v>
+      </c>
+      <c r="C738" t="s">
+        <v>27</v>
+      </c>
+      <c r="D738">
+        <v>9</v>
+      </c>
+      <c r="E738">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="739" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A739" t="s">
+        <v>71</v>
+      </c>
+      <c r="B739" t="s">
+        <v>120</v>
+      </c>
+      <c r="C739" t="s">
+        <v>26</v>
+      </c>
+      <c r="D739">
+        <v>6</v>
+      </c>
+      <c r="E739">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="740" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A740" t="s">
+        <v>66</v>
+      </c>
+      <c r="B740" t="s">
+        <v>109</v>
+      </c>
+      <c r="C740" t="s">
+        <v>24</v>
+      </c>
+      <c r="D740">
+        <v>12.4</v>
+      </c>
+      <c r="E740">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="741" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A741" t="s">
+        <v>66</v>
+      </c>
+      <c r="B741" t="s">
+        <v>106</v>
+      </c>
+      <c r="C741" t="s">
+        <v>22</v>
+      </c>
+      <c r="D741">
+        <v>6.7</v>
+      </c>
+      <c r="E741">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="742" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A742" t="s">
+        <v>66</v>
+      </c>
+      <c r="B742" t="s">
+        <v>118</v>
+      </c>
+      <c r="C742" t="s">
+        <v>22</v>
+      </c>
+      <c r="D742">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E742">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="743" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
+        <v>66</v>
+      </c>
+      <c r="B743" t="s">
+        <v>107</v>
+      </c>
+      <c r="C743" t="s">
+        <v>23</v>
+      </c>
+      <c r="D743">
+        <v>0.9</v>
+      </c>
+      <c r="E743">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="744" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A744" t="s">
+        <v>66</v>
+      </c>
+      <c r="B744" t="s">
+        <v>110</v>
+      </c>
+      <c r="C744" t="s">
+        <v>23</v>
+      </c>
+      <c r="D744">
+        <v>11.8</v>
+      </c>
+      <c r="E744">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="745" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A745" t="s">
+        <v>66</v>
+      </c>
+      <c r="B745" t="s">
+        <v>111</v>
+      </c>
+      <c r="C745" t="s">
+        <v>25</v>
+      </c>
+      <c r="D745">
+        <v>5.3</v>
+      </c>
+      <c r="E745">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="746" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A746" t="s">
+        <v>66</v>
+      </c>
+      <c r="B746" t="s">
+        <v>263</v>
+      </c>
+      <c r="C746" t="s">
+        <v>326</v>
+      </c>
+      <c r="D746">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E746">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="747" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A747" t="s">
+        <v>66</v>
+      </c>
+      <c r="B747" t="s">
+        <v>328</v>
+      </c>
+      <c r="C747" t="s">
+        <v>27</v>
+      </c>
+      <c r="D747">
+        <v>10</v>
+      </c>
+      <c r="E747">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="748" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A748" t="s">
+        <v>66</v>
+      </c>
+      <c r="B748" t="s">
+        <v>340</v>
+      </c>
+      <c r="C748" t="s">
+        <v>26</v>
+      </c>
+      <c r="D748">
+        <v>4</v>
+      </c>
+      <c r="E748">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="749" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A749" t="s">
+        <v>65</v>
+      </c>
+      <c r="B749" t="s">
+        <v>80</v>
+      </c>
+      <c r="C749" t="s">
+        <v>24</v>
+      </c>
+      <c r="D749">
+        <v>24.3</v>
+      </c>
+      <c r="E749">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="750" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A750" t="s">
+        <v>65</v>
+      </c>
+      <c r="B750" t="s">
+        <v>93</v>
+      </c>
+      <c r="C750" t="s">
+        <v>22</v>
+      </c>
+      <c r="D750">
+        <v>18.3</v>
+      </c>
+      <c r="E750">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="751" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A751" t="s">
+        <v>65</v>
+      </c>
+      <c r="B751" t="s">
+        <v>95</v>
+      </c>
+      <c r="C751" t="s">
+        <v>22</v>
+      </c>
+      <c r="D751">
+        <v>25.2</v>
+      </c>
+      <c r="E751">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="752" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A752" t="s">
+        <v>65</v>
+      </c>
+      <c r="B752" t="s">
+        <v>91</v>
+      </c>
+      <c r="C752" t="s">
+        <v>23</v>
+      </c>
+      <c r="D752">
+        <v>19.3</v>
+      </c>
+      <c r="E752">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="753" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A753" t="s">
+        <v>65</v>
+      </c>
+      <c r="B753" t="s">
+        <v>92</v>
+      </c>
+      <c r="C753" t="s">
+        <v>23</v>
+      </c>
+      <c r="D753">
+        <v>0.9</v>
+      </c>
+      <c r="E753">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="754" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A754" t="s">
+        <v>65</v>
+      </c>
+      <c r="B754" t="s">
+        <v>274</v>
+      </c>
+      <c r="C754" t="s">
+        <v>25</v>
+      </c>
+      <c r="D754">
+        <v>5.5</v>
+      </c>
+      <c r="E754">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="755" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A755" t="s">
+        <v>65</v>
+      </c>
+      <c r="B755" t="s">
+        <v>356</v>
+      </c>
+      <c r="C755" t="s">
+        <v>326</v>
+      </c>
+      <c r="D755">
+        <v>8.1</v>
+      </c>
+      <c r="E755">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="756" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A756" t="s">
+        <v>65</v>
+      </c>
+      <c r="B756" t="s">
+        <v>20</v>
+      </c>
+      <c r="C756" t="s">
+        <v>27</v>
+      </c>
+      <c r="D756">
+        <v>-5</v>
+      </c>
+      <c r="E756">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="757" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A757" t="s">
+        <v>65</v>
+      </c>
+      <c r="B757" t="s">
+        <v>296</v>
+      </c>
+      <c r="C757" t="s">
+        <v>26</v>
+      </c>
+      <c r="D757">
+        <v>17</v>
+      </c>
+      <c r="E757">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>